<commit_message>
mis a jour du sprint backlog
</commit_message>
<xml_diff>
--- a/Gestion de projet/3 Product-Sprint Backlog.xlsx
+++ b/Gestion de projet/3 Product-Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\formationJava\Dossier Git\git clone\ProxiBanqueV4\ProxiBanqueV4\Gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7301734F-94F8-4E92-8882-E96216F9B32C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3FD70D65-4265-462D-BE28-E18139B7935B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17925" windowHeight="7740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="7740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story Mapping" sheetId="2" r:id="rId1"/>
@@ -830,6 +830,10 @@
     <xf numFmtId="0" fontId="15" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -857,10 +861,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1941,7 +1941,7 @@
   <dimension ref="A4:O44"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1977,20 +1977,20 @@
       <c r="D5" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="65" t="s">
+      <c r="E5" s="65"/>
+      <c r="F5" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
       <c r="K5" s="43"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="68"/>
-      <c r="N5" s="68"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
       <c r="O5" s="43"/>
     </row>
     <row r="6" spans="2:15" ht="5.45" customHeight="1">
@@ -2054,7 +2054,7 @@
       <c r="O8" s="44"/>
     </row>
     <row r="9" spans="2:15" ht="38.25">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="71" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="45"/>
@@ -2084,7 +2084,7 @@
       <c r="O9" s="43"/>
     </row>
     <row r="10" spans="2:15" ht="6" customHeight="1">
-      <c r="B10" s="70"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="47"/>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
@@ -2100,7 +2100,7 @@
       <c r="O10" s="44"/>
     </row>
     <row r="11" spans="2:15" ht="38.25">
-      <c r="B11" s="70"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="45"/>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
@@ -2122,7 +2122,7 @@
       <c r="O11" s="43"/>
     </row>
     <row r="12" spans="2:15" ht="4.9000000000000004" customHeight="1">
-      <c r="B12" s="70"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="47"/>
       <c r="D12" s="51"/>
       <c r="E12" s="51"/>
@@ -2138,7 +2138,7 @@
       <c r="O12" s="44"/>
     </row>
     <row r="13" spans="2:15" ht="25.5">
-      <c r="B13" s="70"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="45"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
@@ -2158,7 +2158,7 @@
       <c r="O13" s="43"/>
     </row>
     <row r="14" spans="2:15" ht="6" customHeight="1">
-      <c r="B14" s="70"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="45"/>
       <c r="D14" s="57"/>
       <c r="E14" s="57"/>
@@ -2174,7 +2174,7 @@
       <c r="O14" s="43"/>
     </row>
     <row r="15" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B15" s="70"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="45"/>
       <c r="D15" s="57"/>
       <c r="E15" s="57"/>
@@ -2194,7 +2194,7 @@
       <c r="O15" s="43"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B16" s="71"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
@@ -2349,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2371,12 +2371,12 @@
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="30"/>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
     </row>
@@ -2668,8 +2668,8 @@
   </sheetPr>
   <dimension ref="B4:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T65" sqref="T65"/>
+    <sheetView topLeftCell="L25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U60" sqref="U60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5060,12 +5060,10 @@
       <c r="L64" s="10">
         <v>6</v>
       </c>
-      <c r="M64" s="75">
+      <c r="M64" s="66">
         <v>7</v>
       </c>
-      <c r="N64" s="75">
-        <v>8</v>
-      </c>
+      <c r="N64" s="66"/>
     </row>
     <row r="65" spans="2:13" ht="15.75" customHeight="1">
       <c r="B65" s="25"/>

</xml_diff>